<commit_message>
Update station list and map
</commit_message>
<xml_diff>
--- a/station_locs.xlsx
+++ b/station_locs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\Staff\Oeyvind_G\Biolok\biolok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4337A4-E7A2-4130-8C6F-3E635ED2E581}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B75DF7-9443-45C9-B093-C0ED59B4C4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{871D4767-F4A0-44CA-A4B0-E4C9EC08FD48}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{871D4767-F4A0-44CA-A4B0-E4C9EC08FD48}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="2" r:id="rId1"/>
@@ -510,9 +510,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -550,7 +550,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -656,7 +656,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -798,7 +798,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -809,23 +809,23 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.06640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.46484375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.73046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>128</v>
       </c>
@@ -854,7 +854,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>14</v>
       </c>
@@ -883,7 +883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>36</v>
       </c>
@@ -912,7 +912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>42</v>
       </c>
@@ -941,7 +941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>50</v>
       </c>
@@ -970,7 +970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>102</v>
       </c>
@@ -999,7 +999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>107</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>108</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>114</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>118</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>120</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>131</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>141</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>142</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>150</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>155</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>166</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>172</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>182</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>183</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>187</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>191</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>192</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>194</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>195</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>201</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3792</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>10336</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10893</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>12698</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>12706</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>12710</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>12711</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>12712</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>12713</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>12715</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>12721</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>12730</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>12734</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>12735</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>12736</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>15546</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>16131</v>
       </c>

</xml_diff>